<commit_message>
support rhub3.0 and add one new pRRU
</commit_message>
<xml_diff>
--- a/Src/SCMT/tools/RruAntAlarmError/RruAntAlarmError/cfg/器件表.xlsx
+++ b/Src/SCMT/tools/RruAntAlarmError/RruAntAlarmError/cfg/器件表.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="机框" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>5:emb5116|EMB5116</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +69,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>241:bpoi|BPOI板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>243:bpok|BPOK板</t>
+  </si>
+  <si>
+    <t>22:hbpod|HBPOD板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>rHUB2.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -85,10 +96,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>23:hsctd|HSCTD板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>4:mbps25000|25G</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>143:bpog|BPOG板/177:bpoh|BPOH板/241:bpoi|BPOI板/243:bpok|BPOK板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>143:bpog|BPOG板/177:bpoh|BPOH板/241:bpoi|BPOI板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>NULL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -117,22 +140,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pRHB3112V2</t>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0:mbps1250|1.25G/1:mbps2500|2.5G/2:mbps5000|5G</t>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2/4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:mbps1250|1.25G/1:mbps2500|2.5G/2:mbps5000|5G</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -141,6 +157,22 @@
   </si>
   <si>
     <t>3:mbps10000|10G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>177:bpoh|BPOH板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>178:scte|SCTE板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>240:sctf|SCTF板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:hbpod|HBPOD板</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -181,6 +213,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>178:scte|SCTE板/240:sctf|SCTF板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>图形列数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -213,6 +249,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>143:bpog|BPOG板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>类型名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,51 +297,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>143:BPOG板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>177:BPOH板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>178:SCTE板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>240:SCTF板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>241:BPOI板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>243:BPOK板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>22:HBPOD板</t>
-  </si>
-  <si>
-    <t>22:HBPOD板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>23:HSCTD板</t>
-  </si>
-  <si>
-    <t>23:HSCTD板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>178:SCTE板/240:SCTF板</t>
-  </si>
-  <si>
-    <t>143:BPOG板/177:BPOH板/241:BPOI板</t>
-  </si>
-  <si>
-    <t>143:BPOG板/177:BPOH板/241:BPOI板/243:BPOK板</t>
+    <t>rHUB3.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pRHB3112V2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pRHB3112V3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4:mbps25000|25G</t>
+  </si>
+  <si>
+    <t>李弋</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加rHUB3.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:mbps2500|2.5G/1:mbps5000|5G/3:mbps10000|10G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:mbps1250|1.25G/1:mbps2500|2.5G/2:mbps5000|5G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:mbps1250|1.25G/1:mbps2500|2.5G/2:mbps5000|5G/3:mbps10000|10G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -504,15 +536,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,7 +583,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,7 +618,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -801,7 +830,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -818,22 +847,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -856,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -869,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -882,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -895,7 +924,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -908,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -921,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -934,7 +963,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -947,7 +976,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -955,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C10" s="18">
         <v>13</v>
@@ -970,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -983,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -996,7 +1025,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -1009,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
@@ -1022,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -1035,7 +1064,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
@@ -1048,7 +1077,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
@@ -1061,7 +1090,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
@@ -1074,7 +1103,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
@@ -1087,7 +1116,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
@@ -1100,7 +1129,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
@@ -1113,7 +1142,7 @@
         <v>11</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1138,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1158,22 +1187,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -1181,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="18">
         <v>5</v>
@@ -1196,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1209,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1222,7 +1251,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1230,13 +1259,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C5" s="18">
         <v>5</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5" s="18">
         <v>6</v>
@@ -1245,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1258,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1271,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1284,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1297,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1310,7 +1339,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -1318,22 +1347,22 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -1341,22 +1370,22 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3">
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1364,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C13" s="18">
         <v>5</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E13" s="18">
         <v>6</v>
@@ -1379,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1392,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1405,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1418,7 +1447,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1431,7 +1460,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -1444,7 +1473,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
@@ -1452,13 +1481,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="C19" s="18">
         <v>5</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E19" s="18">
         <v>6</v>
@@ -1467,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
@@ -1480,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
@@ -1493,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
@@ -1506,7 +1535,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1519,7 +1548,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -1532,7 +1561,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -1540,13 +1569,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C25" s="18">
         <v>10</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E25" s="18">
         <v>8</v>
@@ -1555,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -1568,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
@@ -1581,7 +1610,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
@@ -1594,7 +1623,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
@@ -1607,7 +1636,7 @@
         <v>4</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
@@ -1620,7 +1649,7 @@
         <v>5</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
@@ -1633,7 +1662,7 @@
         <v>6</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
@@ -1646,7 +1675,7 @@
         <v>7</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
@@ -1654,22 +1683,22 @@
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="C33" s="3">
         <v>10</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1708,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1721,7 +1750,7 @@
     <col min="4" max="4" width="13.875" customWidth="1"/>
     <col min="5" max="5" width="19.875" customWidth="1"/>
     <col min="6" max="6" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="48.875" customWidth="1"/>
+    <col min="7" max="7" width="62.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -1729,22 +1758,22 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -1752,22 +1781,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1775,22 +1804,45 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -1881,7 +1933,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -1889,7 +1941,7 @@
         <v>101</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
@@ -1897,7 +1949,7 @@
         <v>102</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1908,29 +1960,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -1938,13 +1991,27 @@
         <v>43337</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="14">
+        <v>43417</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1957,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>